<commit_message>
Deleted commented code Added line break at the end of files
</commit_message>
<xml_diff>
--- a/Analyzis.xlsx
+++ b/Analyzis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C42148-D775-4CD5-8675-EBAE63E0B1FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7A4D51-CE25-47EC-AE0E-EE4708DA9BE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13779,16 +13779,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:rowOff>138793</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>